<commit_message>
very small file update
</commit_message>
<xml_diff>
--- a/webdownload/files/JustvsZieZo.xlsx
+++ b/webdownload/files/JustvsZieZo.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeppy\OneDrive\Bureaublad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{7C3633A5-072A-46F4-8910-9DACA0B77523}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0DCEA72-C268-47C6-A0DF-63123BCABD69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -225,7 +225,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -410,15 +410,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -452,26 +443,35 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -481,14 +481,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -806,12 +806,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55:H55"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -825,16 +823,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="6"/>
-      <c r="F1" s="4" t="s">
+      <c r="C1" s="32"/>
+      <c r="D1" s="33"/>
+      <c r="F1" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="6"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
@@ -857,19 +855,19 @@
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="16" t="s">
         <v>32</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="16" t="s">
         <v>34</v>
       </c>
       <c r="H3" s="2" t="s">
@@ -877,226 +875,226 @@
       </c>
     </row>
     <row r="4" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="9" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="6" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="G13" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="H13" s="18" t="s">
+      <c r="H13" s="15" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="24"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="27"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="24"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="27"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="20"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="24"/>
+      <c r="B18" s="25"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="27"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="28" t="s">
@@ -1110,108 +1108,108 @@
       <c r="H19" s="30"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="27"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="21"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="27"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="21"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="27"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="21"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="27"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="21"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="27"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="21"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="25"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="27"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="21"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="25"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="27"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="21"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="24"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="27"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="20" t="s">
+      <c r="B28" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="24"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="27"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="25"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="27"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="21"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="28" t="s">
@@ -1225,108 +1223,108 @@
       <c r="H30" s="30"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="25" t="s">
+      <c r="B31" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="27"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="21"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="25" t="s">
+      <c r="B32" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="26"/>
-      <c r="H32" s="27"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="21"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="25" t="s">
+      <c r="B33" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="26"/>
-      <c r="H33" s="27"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="21"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B34" s="25" t="s">
+      <c r="B34" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="27"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="21"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="25" t="s">
+      <c r="B35" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="27"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="21"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="25"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="26"/>
-      <c r="F36" s="26"/>
-      <c r="G36" s="26"/>
-      <c r="H36" s="27"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="21"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="25"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="26"/>
-      <c r="F37" s="26"/>
-      <c r="G37" s="26"/>
-      <c r="H37" s="27"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="21"/>
     </row>
     <row r="38" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="20" t="s">
+      <c r="B38" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="21"/>
-      <c r="H38" s="24"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="27"/>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B39" s="20" t="s">
+      <c r="B39" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="21"/>
-      <c r="H39" s="24"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="26"/>
+      <c r="H39" s="27"/>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="25"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="26"/>
-      <c r="F40" s="26"/>
-      <c r="G40" s="26"/>
-      <c r="H40" s="27"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="21"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" s="28" t="s">
@@ -1340,108 +1338,108 @@
       <c r="H41" s="30"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="25" t="s">
+      <c r="B42" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="C42" s="26"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="26"/>
-      <c r="H42" s="27"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="21"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="25" t="s">
+      <c r="B43" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="C43" s="26"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="26"/>
-      <c r="F43" s="26"/>
-      <c r="G43" s="26"/>
-      <c r="H43" s="27"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="21"/>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="25" t="s">
+      <c r="B44" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C44" s="26"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="26"/>
-      <c r="F44" s="26"/>
-      <c r="G44" s="26"/>
-      <c r="H44" s="27"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="21"/>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B45" s="25" t="s">
+      <c r="B45" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="26"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="26"/>
-      <c r="F45" s="26"/>
-      <c r="G45" s="26"/>
-      <c r="H45" s="27"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="21"/>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B46" s="25" t="s">
+      <c r="B46" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="26"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="26"/>
-      <c r="G46" s="26"/>
-      <c r="H46" s="27"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="21"/>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B47" s="25"/>
-      <c r="C47" s="26"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="26"/>
-      <c r="G47" s="26"/>
-      <c r="H47" s="27"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="21"/>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B48" s="25"/>
-      <c r="C48" s="26"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="26"/>
-      <c r="F48" s="26"/>
-      <c r="G48" s="26"/>
-      <c r="H48" s="27"/>
+      <c r="B48" s="19"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="20"/>
+      <c r="H48" s="21"/>
     </row>
     <row r="49" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="20" t="s">
+      <c r="B49" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="C49" s="21"/>
-      <c r="D49" s="21"/>
-      <c r="E49" s="21"/>
-      <c r="F49" s="21"/>
-      <c r="G49" s="21"/>
-      <c r="H49" s="24"/>
+      <c r="C49" s="26"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="26"/>
+      <c r="F49" s="26"/>
+      <c r="G49" s="26"/>
+      <c r="H49" s="27"/>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B50" s="20" t="s">
+      <c r="B50" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="C50" s="21"/>
-      <c r="D50" s="21"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="21"/>
-      <c r="G50" s="21"/>
-      <c r="H50" s="24"/>
+      <c r="C50" s="26"/>
+      <c r="D50" s="26"/>
+      <c r="E50" s="26"/>
+      <c r="F50" s="26"/>
+      <c r="G50" s="26"/>
+      <c r="H50" s="27"/>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B51" s="25"/>
-      <c r="C51" s="26"/>
-      <c r="D51" s="26"/>
-      <c r="E51" s="26"/>
-      <c r="F51" s="26"/>
-      <c r="G51" s="26"/>
-      <c r="H51" s="27"/>
+      <c r="B51" s="19"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="20"/>
+      <c r="H51" s="21"/>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" s="28" t="s">
@@ -1455,62 +1453,95 @@
       <c r="H52" s="30"/>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B53" s="25" t="s">
+      <c r="B53" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C53" s="26"/>
-      <c r="D53" s="26"/>
-      <c r="E53" s="26"/>
-      <c r="F53" s="26"/>
-      <c r="G53" s="26"/>
-      <c r="H53" s="27"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="20"/>
+      <c r="G53" s="20"/>
+      <c r="H53" s="21"/>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B54" s="25" t="s">
+      <c r="B54" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="C54" s="26"/>
-      <c r="D54" s="26"/>
-      <c r="E54" s="26"/>
-      <c r="F54" s="26"/>
-      <c r="G54" s="26"/>
-      <c r="H54" s="27"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="20"/>
+      <c r="F54" s="20"/>
+      <c r="G54" s="20"/>
+      <c r="H54" s="21"/>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B55" s="25" t="s">
+      <c r="B55" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C55" s="26"/>
-      <c r="D55" s="26"/>
-      <c r="E55" s="26"/>
-      <c r="F55" s="26"/>
-      <c r="G55" s="26"/>
-      <c r="H55" s="27"/>
+      <c r="C55" s="20"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="20"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="20"/>
+      <c r="H55" s="21"/>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B56" s="25" t="s">
+      <c r="B56" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="C56" s="26"/>
-      <c r="D56" s="26"/>
-      <c r="E56" s="26"/>
-      <c r="F56" s="26"/>
-      <c r="G56" s="26"/>
-      <c r="H56" s="27"/>
+      <c r="C56" s="20"/>
+      <c r="D56" s="20"/>
+      <c r="E56" s="20"/>
+      <c r="F56" s="20"/>
+      <c r="G56" s="20"/>
+      <c r="H56" s="21"/>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B57" s="31" t="s">
+      <c r="B57" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="C57" s="32"/>
-      <c r="D57" s="32"/>
-      <c r="E57" s="32"/>
-      <c r="F57" s="32"/>
-      <c r="G57" s="32"/>
-      <c r="H57" s="33"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="23"/>
+      <c r="F57" s="23"/>
+      <c r="G57" s="23"/>
+      <c r="H57" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="B36:H36"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B28:H28"/>
+    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="B32:H32"/>
+    <mergeCell ref="B33:H33"/>
+    <mergeCell ref="B34:H34"/>
+    <mergeCell ref="B35:H35"/>
+    <mergeCell ref="B37:H37"/>
+    <mergeCell ref="B38:H38"/>
+    <mergeCell ref="B39:H39"/>
+    <mergeCell ref="B40:H40"/>
+    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="B43:H43"/>
+    <mergeCell ref="B44:H44"/>
+    <mergeCell ref="B45:H45"/>
+    <mergeCell ref="B46:H46"/>
     <mergeCell ref="B56:H56"/>
     <mergeCell ref="B57:H57"/>
     <mergeCell ref="B47:H47"/>
@@ -1521,40 +1552,7 @@
     <mergeCell ref="B53:H53"/>
     <mergeCell ref="B54:H54"/>
     <mergeCell ref="B55:H55"/>
-    <mergeCell ref="B42:H42"/>
-    <mergeCell ref="B43:H43"/>
-    <mergeCell ref="B44:H44"/>
-    <mergeCell ref="B45:H45"/>
-    <mergeCell ref="B46:H46"/>
     <mergeCell ref="B49:H49"/>
-    <mergeCell ref="B37:H37"/>
-    <mergeCell ref="B38:H38"/>
-    <mergeCell ref="B39:H39"/>
-    <mergeCell ref="B40:H40"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="B32:H32"/>
-    <mergeCell ref="B33:H33"/>
-    <mergeCell ref="B34:H34"/>
-    <mergeCell ref="B35:H35"/>
-    <mergeCell ref="B36:H36"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="B30:H30"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="B17:H17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>